<commit_message>
Add folder with tescases
</commit_message>
<xml_diff>
--- a/vtymchyshyn/TestCases.xlsx
+++ b/vtymchyshyn/TestCases.xlsx
@@ -343,9 +343,6 @@
     <t>Verify Quantity Dropdown</t>
   </si>
   <si>
-    <t xml:space="preserve">2. User input valid item number </t>
-  </si>
-  <si>
     <t>2. Select any item</t>
   </si>
   <si>
@@ -356,6 +353,9 @@
   </si>
   <si>
     <t xml:space="preserve"> - System adds  Items to Cart </t>
+  </si>
+  <si>
+    <t>2. User input valid item numbers</t>
   </si>
 </sst>
 </file>
@@ -547,6 +547,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -559,18 +583,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -578,16 +590,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -603,15 +612,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -974,16 +974,16 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="19"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="21"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -992,78 +992,73 @@
       <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="21"/>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="19"/>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="29"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="27"/>
+      <c r="B12" s="31"/>
     </row>
     <row r="13" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="29"/>
+      <c r="B13" s="23"/>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="23"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="23"/>
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="31"/>
+      <c r="B16" s="25"/>
     </row>
     <row r="17" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="27"/>
     </row>
     <row r="18" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="27"/>
     </row>
     <row r="19" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="19"/>
+      <c r="B19" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A11:B11"/>
@@ -1072,6 +1067,11 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1132,76 +1132,76 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="19"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="21"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="19"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="34"/>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="29"/>
     </row>
     <row r="11" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="29"/>
     </row>
     <row r="12" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="29"/>
+      <c r="B12" s="23"/>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="21"/>
+      <c r="B13" s="29"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="36"/>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="38"/>
     </row>
     <row r="16" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="27"/>
     </row>
     <row r="17" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="36"/>
+      <c r="B17" s="39"/>
     </row>
     <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
@@ -1252,76 +1252,76 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="25"/>
+      <c r="B25" s="19"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="21"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="25"/>
+      <c r="B27" s="19"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="34"/>
     </row>
     <row r="29" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="21"/>
+      <c r="B29" s="29"/>
     </row>
     <row r="30" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="21"/>
+      <c r="B30" s="29"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="29"/>
+      <c r="B31" s="23"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="21"/>
+      <c r="B32" s="29"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="33"/>
+      <c r="B33" s="36"/>
     </row>
     <row r="34" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="35"/>
+      <c r="B34" s="38"/>
     </row>
     <row r="35" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="27"/>
     </row>
     <row r="36" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="36"/>
+      <c r="B36" s="39"/>
     </row>
     <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -1362,40 +1362,40 @@
       <c r="B43" s="1"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="25"/>
+      <c r="B44" s="19"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="21"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
+      <c r="A46" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="25"/>
+      <c r="B46" s="19"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="38"/>
+      <c r="B47" s="34"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="21"/>
+      <c r="B48" s="29"/>
     </row>
     <row r="49" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="33"/>
+      <c r="B49" s="36"/>
     </row>
     <row r="50" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="40" t="s">
@@ -1452,76 +1452,76 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="25"/>
+      <c r="B58" s="19"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B59" s="23"/>
+      <c r="B59" s="21"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B60" s="25"/>
+      <c r="B60" s="19"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="37" t="s">
+      <c r="A61" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B61" s="38"/>
+      <c r="B61" s="34"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="39" t="s">
+      <c r="A62" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B62" s="21"/>
+      <c r="B62" s="29"/>
     </row>
     <row r="63" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="21"/>
+      <c r="B63" s="29"/>
     </row>
     <row r="64" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B64" s="29"/>
+      <c r="B64" s="23"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="39" t="s">
+      <c r="A65" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B65" s="21"/>
+      <c r="B65" s="29"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="32" t="s">
+      <c r="A66" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="33"/>
+      <c r="B66" s="36"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="34" t="s">
+      <c r="A67" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B67" s="35"/>
+      <c r="B67" s="38"/>
     </row>
     <row r="68" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
+      <c r="A68" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B68" s="19"/>
+      <c r="B68" s="27"/>
     </row>
     <row r="69" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="36" t="s">
+      <c r="A69" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B69" s="36"/>
+      <c r="B69" s="39"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
@@ -1564,76 +1564,76 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="24" t="s">
+      <c r="A77" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B77" s="25"/>
+      <c r="B77" s="19"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="22" t="s">
+      <c r="A78" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B78" s="23"/>
+      <c r="B78" s="21"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="24" t="s">
+      <c r="A79" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="25"/>
+      <c r="B79" s="19"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="37" t="s">
+      <c r="A80" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B80" s="38"/>
+      <c r="B80" s="34"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="39" t="s">
+      <c r="A81" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B81" s="21"/>
+      <c r="B81" s="29"/>
     </row>
     <row r="82" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="39" t="s">
+      <c r="A82" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B82" s="21"/>
+      <c r="B82" s="29"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="s">
+      <c r="A83" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B83" s="29"/>
+      <c r="B83" s="23"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="39" t="s">
+      <c r="A84" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B84" s="21"/>
+      <c r="B84" s="29"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="32" t="s">
+      <c r="A85" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="33"/>
+      <c r="B85" s="36"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="34" t="s">
+      <c r="A86" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B86" s="35"/>
+      <c r="B86" s="38"/>
     </row>
     <row r="87" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="18" t="s">
+      <c r="A87" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B87" s="19"/>
+      <c r="B87" s="27"/>
     </row>
     <row r="88" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="36" t="s">
+      <c r="A88" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B88" s="36"/>
+      <c r="B88" s="39"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
@@ -1676,93 +1676,120 @@
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="24" t="s">
+      <c r="A96" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B96" s="25"/>
+      <c r="B96" s="19"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="22" t="s">
+      <c r="A97" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B97" s="23"/>
+      <c r="B97" s="21"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="24" t="s">
+      <c r="A98" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B98" s="25"/>
+      <c r="B98" s="19"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="37" t="s">
+      <c r="A99" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B99" s="38"/>
+      <c r="B99" s="34"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="39" t="s">
+      <c r="A100" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B100" s="21"/>
+      <c r="B100" s="29"/>
     </row>
     <row r="101" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="39" t="s">
+      <c r="A101" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B101" s="21"/>
+      <c r="B101" s="29"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="28" t="s">
+      <c r="A102" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B102" s="29"/>
+      <c r="B102" s="23"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="39" t="s">
+      <c r="A103" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B103" s="21"/>
+      <c r="B103" s="29"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="32" t="s">
+      <c r="A104" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B104" s="33"/>
+      <c r="B104" s="36"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="34" t="s">
+      <c r="A105" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B105" s="35"/>
+      <c r="B105" s="38"/>
     </row>
     <row r="106" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="18" t="s">
+      <c r="A106" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B106" s="19"/>
+      <c r="B106" s="27"/>
     </row>
     <row r="107" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="36" t="s">
+      <c r="A107" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B107" s="36"/>
+      <c r="B107" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
@@ -1775,47 +1802,20 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1874,40 +1874,40 @@
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="19"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="21"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="19"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="34"/>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="33"/>
+      <c r="B10" s="36"/>
     </row>
     <row r="11" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="28"/>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
@@ -1961,7 +1961,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2009,64 +2009,64 @@
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="19"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="33" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="48"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="21"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="34"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="25"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="B11" s="29"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="38"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="21"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="29"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="33"/>
+      <c r="B13" s="36"/>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="46"/>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="39"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>

</xml_diff>